<commit_message>
Updates to module functions
</commit_message>
<xml_diff>
--- a/inst/extdata/controlTables.xlsx
+++ b/inst/extdata/controlTables.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EC0D72-74B5-4641-9E26-701CB65A8945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCED295-96B8-493E-BD93-752BD8D3406F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -1563,7 +1563,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="45">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1815,6 +1815,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -2048,7 +2054,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2201,6 +2207,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="13" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="9" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="63">
     <cellStyle name="20% - Accent1" xfId="33" builtinId="30" customBuiltin="1"/>
@@ -2269,6 +2277,163 @@
   </cellStyles>
   <dxfs count="157">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
@@ -3482,80 +3647,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -4074,89 +4165,6 @@
         <scheme val="minor"/>
       </font>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5495,115 +5503,115 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DFE6321-7DE3-4183-8A83-7F36C85C9DB0}" name="co_slrCm" displayName="co_slrCm" ref="B79:E86" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DFE6321-7DE3-4183-8A83-7F36C85C9DB0}" name="co_slrCm" displayName="co_slrCm" ref="B79:E86" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3762ECAE-6A4D-4316-A236-8B365D0626D2}" name="row_id" dataDxfId="71">
+    <tableColumn id="1" xr3:uid="{3762ECAE-6A4D-4316-A236-8B365D0626D2}" name="row_id" dataDxfId="78">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_slrCm[[#This Row],[row_id]] ) - ROW( co_slrCm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{652FAEDD-ACCA-4F89-BB09-D0259DE4EBDE}" name="model" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{4E21FF99-5816-430F-A59C-839B9DED59AD}" name="model_cm" dataDxfId="69">
+    <tableColumn id="2" xr3:uid="{652FAEDD-ACCA-4F89-BB09-D0259DE4EBDE}" name="model" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{4E21FF99-5816-430F-A59C-839B9DED59AD}" name="model_cm" dataDxfId="76">
       <calculatedColumnFormula xml:space="preserve"> SUBSTITUTE( co_slrCm[[#This Row],[model]], "cm", "" )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{494DF020-2C7F-4BEC-BF92-2D1C2997DB71}" name="model_type" dataDxfId="68"/>
+    <tableColumn id="20" xr3:uid="{494DF020-2C7F-4BEC-BF92-2D1C2997DB71}" name="model_type" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D0C88C5-F2A7-46B8-8C69-B1B5A09A785D}" name="co_moduleAreas" displayName="co_moduleAreas" ref="B147:G151" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D0C88C5-F2A7-46B8-8C69-B1B5A09A785D}" name="co_moduleAreas" displayName="co_moduleAreas" ref="B147:G151" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6B39C0F6-F51F-46E7-B871-D79691468859}" name="row_id" dataDxfId="65">
+    <tableColumn id="1" xr3:uid="{6B39C0F6-F51F-46E7-B871-D79691468859}" name="row_id" dataDxfId="72">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleAreas[[#This Row],[row_id]] ) - ROW( co_moduleAreas[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FA7D71D8-3E5E-4160-8B14-D5765D9F310B}" name="module" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{FF99F0AF-3896-4181-B4BA-A7BCCD26281F}" name="CONUS" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{8D6CF49E-2833-4B79-B861-B3E559469D80}" name="AK" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{FBF0E9DC-EC64-4AAB-85A0-909CE7D91B5C}" name="HI" dataDxfId="61"/>
-    <tableColumn id="6" xr3:uid="{ECDD11B8-8AA9-466D-9A95-87825C1F011B}" name="US" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{FA7D71D8-3E5E-4160-8B14-D5765D9F310B}" name="module" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{FF99F0AF-3896-4181-B4BA-A7BCCD26281F}" name="CONUS" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{8D6CF49E-2833-4B79-B861-B3E559469D80}" name="AK" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{FBF0E9DC-EC64-4AAB-85A0-909CE7D91B5C}" name="HI" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{ECDD11B8-8AA9-466D-9A95-87825C1F011B}" name="US" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A7B7951-C6F2-4FD3-A1BB-7026F6A8E846}" name="co_areas" displayName="co_areas" ref="B138:E142" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A7B7951-C6F2-4FD3-A1BB-7026F6A8E846}" name="co_areas" displayName="co_areas" ref="B138:E142" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B139:E142">
     <sortCondition ref="E139:E142"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7EF0B14-6E39-4AC7-AF6C-1F6122F80A00}" name="row_id" dataDxfId="57">
+    <tableColumn id="1" xr3:uid="{E7EF0B14-6E39-4AC7-AF6C-1F6122F80A00}" name="row_id" dataDxfId="64">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_areas[[#This Row],[row_id]] ) - ROW( co_areas[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8E314417-76FC-49D4-8395-68E6821400F1}" name="area" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{D3346EB3-CC6E-4F56-99C1-5CA14B2AA885}" name="area_label" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{49EF0AA8-E61C-4619-9F0A-C99D809CE4D7}" name="area_order" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{8E314417-76FC-49D4-8395-68E6821400F1}" name="area" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{D3346EB3-CC6E-4F56-99C1-5CA14B2AA885}" name="area_label" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{49EF0AA8-E61C-4619-9F0A-C99D809CE4D7}" name="area_order" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{130DC324-CB3E-4D07-B21F-C092D038DD02}" name="co_moduleScenarios" displayName="co_moduleScenarios" ref="B122:G129" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{130DC324-CB3E-4D07-B21F-C092D038DD02}" name="co_moduleScenarios" displayName="co_moduleScenarios" ref="B122:G129" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{153273EE-D49C-43E7-89D3-640CF711FDD6}" name="row_id" dataDxfId="51">
+    <tableColumn id="1" xr3:uid="{153273EE-D49C-43E7-89D3-640CF711FDD6}" name="row_id" dataDxfId="58">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleScenarios[[#This Row],[row_id]] ) - ROW( co_moduleScenarios[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F54B7C7D-6137-4D7A-AA53-E6EC1A4D870B}" name="inputType" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{8C7B1E0B-A838-4C25-BD81-F2D99A20C316}" name="fredi" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{DE883AA6-AFB1-4ECB-81BC-2DBBBB7D9EC6}" name="sv" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{03493EE6-57B6-434B-89CB-00D18647CE1C}" name="extremes" dataDxfId="47"/>
-    <tableColumn id="6" xr3:uid="{FD0E66B9-364C-46F1-A441-3593D5002F5F}" name="ghg" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{F54B7C7D-6137-4D7A-AA53-E6EC1A4D870B}" name="inputType" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{8C7B1E0B-A838-4C25-BD81-F2D99A20C316}" name="fredi" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{DE883AA6-AFB1-4ECB-81BC-2DBBBB7D9EC6}" name="sv" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{03493EE6-57B6-434B-89CB-00D18647CE1C}" name="extremes" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{FD0E66B9-364C-46F1-A441-3593D5002F5F}" name="ghg" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}" name="co_moduleInfo" displayName="co_moduleInfo" ref="B22:G26" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}" name="co_moduleInfo" displayName="co_moduleInfo" ref="B22:G26" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="B22:G26" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B23:G25">
     <sortCondition ref="C33:C35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1E91507F-C783-4AF1-A2DC-F0D550DB8228}" name="row_id" dataDxfId="43" totalsRowDxfId="42">
+    <tableColumn id="1" xr3:uid="{1E91507F-C783-4AF1-A2DC-F0D550DB8228}" name="row_id" dataDxfId="50" totalsRowDxfId="49">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleInfo[[#This Row],[row_id]] ) - ROW(co_moduleInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C5A172CB-7A1A-40A6-B5FF-ADA60A854570}" name="module" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{40CB1771-C104-47EE-A9D3-FC2266D98E31}" name="defaultMinYr" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{361574C9-CD04-4844-8EA4-8686C22861AF}" name="defaultMaxYr" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{BE556F7A-79ED-4CF4-9DE1-89B19E392F66}" name="moduleMinYr" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{EE868D0F-708E-48BF-843C-D20D3F01FC0A}" name="moduleMaxYr" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{C5A172CB-7A1A-40A6-B5FF-ADA60A854570}" name="module" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{40CB1771-C104-47EE-A9D3-FC2266D98E31}" name="defaultMinYr" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{361574C9-CD04-4844-8EA4-8686C22861AF}" name="defaultMaxYr" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{BE556F7A-79ED-4CF4-9DE1-89B19E392F66}" name="moduleMinYr" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{EE868D0F-708E-48BF-843C-D20D3F01FC0A}" name="moduleMaxYr" dataDxfId="40" totalsRowDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3617F852-F5F0-4F60-AE1D-02F268E7E5D0}" name="co_moduleModTypes" displayName="co_moduleModTypes" ref="B69:F73" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3617F852-F5F0-4F60-AE1D-02F268E7E5D0}" name="co_moduleModTypes" displayName="co_moduleModTypes" ref="B69:F73" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B2363595-A68F-4CF5-9F7E-DD47303CE84C}" name="row_id" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{B2363595-A68F-4CF5-9F7E-DD47303CE84C}" name="row_id" dataDxfId="36">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleModTypes[[#This Row],[row_id]] ) - ROW( co_moduleModTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D18390C5-26C7-473C-9856-A402FD3A0AEF}" name="module" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{C4E5B6A3-7C3C-4259-823B-02A74FE928D8}" name="gcm" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{F47429F2-FAE8-479B-9DBC-65A9498A8337}" name="slr" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{935107B0-7729-4F94-B463-7640686C80D6}" name="gcm_ghg" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{D18390C5-26C7-473C-9856-A402FD3A0AEF}" name="module" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{C4E5B6A3-7C3C-4259-823B-02A74FE928D8}" name="gcm" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{F47429F2-FAE8-479B-9DBC-65A9498A8337}" name="slr" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{935107B0-7729-4F94-B463-7640686C80D6}" name="gcm_ghg" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{826DC812-3005-4F51-B0FF-C3E353D9AAA4}" name="co_scenarios" displayName="co_scenarios" ref="B104:F116" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{826DC812-3005-4F51-B0FF-C3E353D9AAA4}" name="co_scenarios" displayName="co_scenarios" ref="B104:F116" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6346090C-91C3-4EDB-A7F1-370F8A29D56E}" name="row_id" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{6346090C-91C3-4EDB-A7F1-370F8A29D56E}" name="row_id" dataDxfId="29">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_scenarios[[#This Row],[row_id]] ) - ROW( co_scenarios[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF567B04-BAFE-4398-9598-BABE0A898EC3}" name="scenarioName" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{11EC5AD1-152B-4E01-89B5-BF7C4B3D34E7}" name="inputName" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{713CE323-B977-4F6A-A751-4F21E1A47B9D}" name="inputArgType" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{A3EF825F-7245-45C7-97D2-FB17A58B2688}" name="inputArgVal" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{AF567B04-BAFE-4398-9598-BABE0A898EC3}" name="scenarioName" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{11EC5AD1-152B-4E01-89B5-BF7C4B3D34E7}" name="inputName" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{713CE323-B977-4F6A-A751-4F21E1A47B9D}" name="inputArgType" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{A3EF825F-7245-45C7-97D2-FB17A58B2688}" name="inputArgVal" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5613,10 +5621,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}" name="Readme_adaptations" displayName="Readme_adaptations" ref="B9:E15" totalsRowShown="0">
   <autoFilter ref="B9:E15" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="24">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_adaptations[[#This Row],[row_id]] ) - ROW( Readme_adaptations[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{13712644-0D89-49D5-9571-32BD03BF1BD3}" name="adapt_id"/>
     <tableColumn id="3" xr3:uid="{B89736B7-3040-4F82-B2CC-EB15F47F50B3}" name="adapt_label"/>
   </tableColumns>
@@ -5625,16 +5633,16 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="B3:F5" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="20">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_sectors[[#This Row],[row_id]] ) - ROW( Readme_sectors[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5644,17 +5652,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}" name="slr_cm" displayName="slr_cm" ref="A1:I102" totalsRowShown="0">
   <autoFilter ref="A1:I102" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="15">
       <calculatedColumnFormula xml:space="preserve"> ROW( slr_cm[[#This Row],[row_id]] ) - ROW( slr_cm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5759,75 +5767,75 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarTypes" displayName="co_scalarTypes" ref="B42:C47" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarTypes" displayName="co_scalarTypes" ref="B42:C47" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="B42:C47" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B43:C47">
     <sortCondition ref="C43:C47"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="102">
+    <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="1">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_scalarTypes[[#This Row],[row_id]] ) - ROW( co_scalarTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{057C556C-4A5B-41BF-9EA5-CD5D06EC20A3}" name="scalarType" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{057C556C-4A5B-41BF-9EA5-CD5D06EC20A3}" name="scalarType" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B52:E55" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B52:E55" totalsRowShown="0" headerRowDxfId="104" dataDxfId="103">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="98">
+    <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="102">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{76AF9F40-EEBA-4ABF-82CC-7580151C94E2}" name="econMultiplierName" dataDxfId="97"/>
-    <tableColumn id="3" xr3:uid="{BB4C0E23-5864-41DA-8215-7C526A80B49B}" name="econMultiplierLabel" dataDxfId="96"/>
-    <tableColumn id="2" xr3:uid="{013806BA-C4E3-46FD-AD7B-D198CFA696CD}" name="valueYear" dataDxfId="95"/>
+    <tableColumn id="4" xr3:uid="{76AF9F40-EEBA-4ABF-82CC-7580151C94E2}" name="econMultiplierName" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{BB4C0E23-5864-41DA-8215-7C526A80B49B}" name="econMultiplierLabel" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{013806BA-C4E3-46FD-AD7B-D198CFA696CD}" name="valueYear" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B92:L99" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B92:L99" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="92">
+    <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="96">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{45198473-3D48-41CD-B663-D0AF13813C66}" name="inputName" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{E3847F4D-6384-49D5-8156-9EC8E8221B62}" name="inputType" dataDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{F9249B62-F8E8-46B3-88F1-E8E0903FDD4A}" name="inputUnit" dataDxfId="89"/>
-    <tableColumn id="6" xr3:uid="{48BBD66A-C5AD-477C-84C9-E5FFE0D43B87}" name="inputMin" dataDxfId="88"/>
-    <tableColumn id="7" xr3:uid="{05D78FF1-5FB5-4CB5-AB55-8F3089B354DC}" name="inputMax" dataDxfId="87">
+    <tableColumn id="4" xr3:uid="{45198473-3D48-41CD-B663-D0AF13813C66}" name="inputName" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{E3847F4D-6384-49D5-8156-9EC8E8221B62}" name="inputType" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{F9249B62-F8E8-46B3-88F1-E8E0903FDD4A}" name="inputUnit" dataDxfId="93"/>
+    <tableColumn id="6" xr3:uid="{48BBD66A-C5AD-477C-84C9-E5FFE0D43B87}" name="inputMin" dataDxfId="92"/>
+    <tableColumn id="7" xr3:uid="{05D78FF1-5FB5-4CB5-AB55-8F3089B354DC}" name="inputMax" dataDxfId="91">
       <calculatedColumnFormula xml:space="preserve"> IF( ISNA( MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ), "", INDEX( co_modelTypes[driverMaxOutput], MATCH( co_inputInfo[[#This Row],[inputType]], co_modelTypes[inputName], 0 ) ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{529C7942-976A-4B70-B5DE-FAD89A0065FC}" name="refYear" dataDxfId="86"/>
-    <tableColumn id="11" xr3:uid="{33838F63-5751-4209-AF1E-14DFB927DF2E}" name="minYear" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{1C94F8DC-2CA2-47FD-A5E1-761F8E67704A}" name="valueCol" dataDxfId="84"/>
-    <tableColumn id="5" xr3:uid="{99885E6A-BA0C-4550-ACB2-9BF751DC0F7C}" name="valueColLC" dataDxfId="83">
+    <tableColumn id="10" xr3:uid="{529C7942-976A-4B70-B5DE-FAD89A0065FC}" name="refYear" dataDxfId="90"/>
+    <tableColumn id="11" xr3:uid="{33838F63-5751-4209-AF1E-14DFB927DF2E}" name="minYear" dataDxfId="89"/>
+    <tableColumn id="8" xr3:uid="{1C94F8DC-2CA2-47FD-A5E1-761F8E67704A}" name="valueCol" dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{99885E6A-BA0C-4550-ACB2-9BF751DC0F7C}" name="valueColLC" dataDxfId="87">
       <calculatedColumnFormula xml:space="preserve"> LOWER( co_inputInfo[[#This Row],[valueCol]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="regional" dataDxfId="82"/>
+    <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="regional" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B173:H225" totalsRowShown="0" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B173:H225" totalsRowShown="0" headerRowDxfId="85">
   <autoFilter ref="B173:H225" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="80">
+    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="84">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{75C24D34-7FF1-4D85-8B86-75A1F1B7EF6C}" name="region" dataDxfId="76"/>
-    <tableColumn id="7" xr3:uid="{B0056655-B67E-486D-8580-C33D8B965DEB}" name="area" dataDxfId="75">
+    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="82"/>
+    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="81"/>
+    <tableColumn id="6" xr3:uid="{75C24D34-7FF1-4D85-8B86-75A1F1B7EF6C}" name="region" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{B0056655-B67E-486D-8580-C33D8B965DEB}" name="area" dataDxfId="4">
       <calculatedColumnFormula array="1" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FD967E7F-5A29-4247-8725-12F353B23771}" name="state_order" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{FD967E7F-5A29-4247-8725-12F353B23771}" name="state_order" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7242,9 +7250,9 @@
   </sheetPr>
   <dimension ref="A1:U225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J99" sqref="J99"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9489,7 +9497,7 @@
       <c r="F174" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G174" s="48" t="str" cm="1">
+      <c r="G174" s="60" t="str" cm="1">
         <f t="array" ref="G174" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9514,7 +9522,7 @@
       <c r="F175" s="49" t="s">
         <v>276</v>
       </c>
-      <c r="G175" s="49" t="str" cm="1">
+      <c r="G175" s="61" t="str" cm="1">
         <f t="array" ref="G175" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>AK</v>
       </c>
@@ -9539,7 +9547,7 @@
       <c r="F176" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="G176" s="48" t="str" cm="1">
+      <c r="G176" s="60" t="str" cm="1">
         <f t="array" ref="G176" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9564,7 +9572,7 @@
       <c r="F177" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G177" s="48" t="str" cm="1">
+      <c r="G177" s="60" t="str" cm="1">
         <f t="array" ref="G177" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9589,7 +9597,7 @@
       <c r="F178" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="G178" s="48" t="str" cm="1">
+      <c r="G178" s="60" t="str" cm="1">
         <f t="array" ref="G178" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9614,7 +9622,7 @@
       <c r="F179" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="G179" s="48" t="str" cm="1">
+      <c r="G179" s="60" t="str" cm="1">
         <f t="array" ref="G179" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9639,7 +9647,7 @@
       <c r="F180" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G180" s="48" t="str" cm="1">
+      <c r="G180" s="60" t="str" cm="1">
         <f t="array" ref="G180" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9664,7 +9672,7 @@
       <c r="F181" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G181" s="48" t="str" cm="1">
+      <c r="G181" s="60" t="str" cm="1">
         <f t="array" ref="G181" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9689,7 +9697,7 @@
       <c r="F182" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G182" s="48" t="str" cm="1">
+      <c r="G182" s="60" t="str" cm="1">
         <f t="array" ref="G182" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9714,7 +9722,7 @@
       <c r="F183" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G183" s="48" t="str" cm="1">
+      <c r="G183" s="60" t="str" cm="1">
         <f t="array" ref="G183" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9739,7 +9747,7 @@
       <c r="F184" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G184" s="48" t="str" cm="1">
+      <c r="G184" s="60" t="str" cm="1">
         <f t="array" ref="G184" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9764,7 +9772,7 @@
       <c r="F185" s="49" t="s">
         <v>277</v>
       </c>
-      <c r="G185" s="49" t="str" cm="1">
+      <c r="G185" s="61" t="str" cm="1">
         <f t="array" ref="G185" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>HI</v>
       </c>
@@ -9789,7 +9797,7 @@
       <c r="F186" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="G186" s="48" t="str" cm="1">
+      <c r="G186" s="60" t="str" cm="1">
         <f t="array" ref="G186" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9814,7 +9822,7 @@
       <c r="F187" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G187" s="48" t="str" cm="1">
+      <c r="G187" s="60" t="str" cm="1">
         <f t="array" ref="G187" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9839,7 +9847,7 @@
       <c r="F188" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G188" s="48" t="str" cm="1">
+      <c r="G188" s="60" t="str" cm="1">
         <f t="array" ref="G188" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9864,7 +9872,7 @@
       <c r="F189" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G189" s="48" t="str" cm="1">
+      <c r="G189" s="60" t="str" cm="1">
         <f t="array" ref="G189" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9889,7 +9897,7 @@
       <c r="F190" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="G190" s="48" t="str" cm="1">
+      <c r="G190" s="60" t="str" cm="1">
         <f t="array" ref="G190" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9914,7 +9922,7 @@
       <c r="F191" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G191" s="48" t="str" cm="1">
+      <c r="G191" s="60" t="str" cm="1">
         <f t="array" ref="G191" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9939,7 +9947,7 @@
       <c r="F192" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G192" s="48" t="str" cm="1">
+      <c r="G192" s="60" t="str" cm="1">
         <f t="array" ref="G192" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9964,7 +9972,7 @@
       <c r="F193" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G193" s="48" t="str" cm="1">
+      <c r="G193" s="60" t="str" cm="1">
         <f t="array" ref="G193" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -9989,7 +9997,7 @@
       <c r="F194" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G194" s="48" t="str" cm="1">
+      <c r="G194" s="60" t="str" cm="1">
         <f t="array" ref="G194" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10014,7 +10022,7 @@
       <c r="F195" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G195" s="48" t="str" cm="1">
+      <c r="G195" s="60" t="str" cm="1">
         <f t="array" ref="G195" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10039,7 +10047,7 @@
       <c r="F196" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G196" s="48" t="str" cm="1">
+      <c r="G196" s="60" t="str" cm="1">
         <f t="array" ref="G196" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10064,7 +10072,7 @@
       <c r="F197" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G197" s="48" t="str" cm="1">
+      <c r="G197" s="60" t="str" cm="1">
         <f t="array" ref="G197" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10089,7 +10097,7 @@
       <c r="F198" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G198" s="48" t="str" cm="1">
+      <c r="G198" s="60" t="str" cm="1">
         <f t="array" ref="G198" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10114,7 +10122,7 @@
       <c r="F199" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G199" s="48" t="str" cm="1">
+      <c r="G199" s="60" t="str" cm="1">
         <f t="array" ref="G199" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10139,7 +10147,7 @@
       <c r="F200" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="G200" s="48" t="str" cm="1">
+      <c r="G200" s="60" t="str" cm="1">
         <f t="array" ref="G200" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10164,7 +10172,7 @@
       <c r="F201" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="G201" s="48" t="str" cm="1">
+      <c r="G201" s="60" t="str" cm="1">
         <f t="array" ref="G201" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10189,7 +10197,7 @@
       <c r="F202" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="G202" s="48" t="str" cm="1">
+      <c r="G202" s="60" t="str" cm="1">
         <f t="array" ref="G202" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10214,7 +10222,7 @@
       <c r="F203" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G203" s="48" t="str" cm="1">
+      <c r="G203" s="60" t="str" cm="1">
         <f t="array" ref="G203" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10239,7 +10247,7 @@
       <c r="F204" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G204" s="48" t="str" cm="1">
+      <c r="G204" s="60" t="str" cm="1">
         <f t="array" ref="G204" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10264,7 +10272,7 @@
       <c r="F205" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="G205" s="48" t="str" cm="1">
+      <c r="G205" s="60" t="str" cm="1">
         <f t="array" ref="G205" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10289,7 +10297,7 @@
       <c r="F206" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G206" s="48" t="str" cm="1">
+      <c r="G206" s="60" t="str" cm="1">
         <f t="array" ref="G206" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10314,7 +10322,7 @@
       <c r="F207" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G207" s="48" t="str" cm="1">
+      <c r="G207" s="60" t="str" cm="1">
         <f t="array" ref="G207" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10339,7 +10347,7 @@
       <c r="F208" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="G208" s="48" t="str" cm="1">
+      <c r="G208" s="60" t="str" cm="1">
         <f t="array" ref="G208" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10364,7 +10372,7 @@
       <c r="F209" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G209" s="48" t="str" cm="1">
+      <c r="G209" s="60" t="str" cm="1">
         <f t="array" ref="G209" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10389,7 +10397,7 @@
       <c r="F210" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="G210" s="48" t="str" cm="1">
+      <c r="G210" s="60" t="str" cm="1">
         <f t="array" ref="G210" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10414,7 +10422,7 @@
       <c r="F211" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="G211" s="48" t="str" cm="1">
+      <c r="G211" s="60" t="str" cm="1">
         <f t="array" ref="G211" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10439,7 +10447,7 @@
       <c r="F212" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G212" s="48" t="str" cm="1">
+      <c r="G212" s="60" t="str" cm="1">
         <f t="array" ref="G212" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10464,7 +10472,7 @@
       <c r="F213" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G213" s="48" t="str" cm="1">
+      <c r="G213" s="60" t="str" cm="1">
         <f t="array" ref="G213" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10489,7 +10497,7 @@
       <c r="F214" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G214" s="48" t="str" cm="1">
+      <c r="G214" s="60" t="str" cm="1">
         <f t="array" ref="G214" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10514,7 +10522,7 @@
       <c r="F215" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="G215" s="48" t="str" cm="1">
+      <c r="G215" s="60" t="str" cm="1">
         <f t="array" ref="G215" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10539,7 +10547,7 @@
       <c r="F216" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G216" s="48" t="str" cm="1">
+      <c r="G216" s="60" t="str" cm="1">
         <f t="array" ref="G216" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10564,7 +10572,7 @@
       <c r="F217" s="48" t="s">
         <v>274</v>
       </c>
-      <c r="G217" s="48" t="str" cm="1">
+      <c r="G217" s="60" t="str" cm="1">
         <f t="array" ref="G217" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10589,7 +10597,7 @@
       <c r="F218" s="48" t="s">
         <v>275</v>
       </c>
-      <c r="G218" s="48" t="str" cm="1">
+      <c r="G218" s="60" t="str" cm="1">
         <f t="array" ref="G218" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10614,7 +10622,7 @@
       <c r="F219" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G219" s="48" t="str" cm="1">
+      <c r="G219" s="60" t="str" cm="1">
         <f t="array" ref="G219" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10639,7 +10647,7 @@
       <c r="F220" s="48" t="s">
         <v>273</v>
       </c>
-      <c r="G220" s="48" t="str" cm="1">
+      <c r="G220" s="60" t="str" cm="1">
         <f t="array" ref="G220" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10664,7 +10672,7 @@
       <c r="F221" s="48" t="s">
         <v>272</v>
       </c>
-      <c r="G221" s="48" t="str" cm="1">
+      <c r="G221" s="60" t="str" cm="1">
         <f t="array" ref="G221" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10689,7 +10697,7 @@
       <c r="F222" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="G222" s="48" t="str" cm="1">
+      <c r="G222" s="60" t="str" cm="1">
         <f t="array" ref="G222" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10714,7 +10722,7 @@
       <c r="F223" s="48" t="s">
         <v>270</v>
       </c>
-      <c r="G223" s="48" t="str" cm="1">
+      <c r="G223" s="60" t="str" cm="1">
         <f t="array" ref="G223" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10739,7 +10747,7 @@
       <c r="F224" s="48" t="s">
         <v>271</v>
       </c>
-      <c r="G224" s="48" t="str" cm="1">
+      <c r="G224" s="60" t="str" cm="1">
         <f t="array" ref="G224" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>CONUS</v>
       </c>
@@ -10764,7 +10772,7 @@
       <c r="F225" s="49" t="s">
         <v>280</v>
       </c>
-      <c r="G225" s="49" t="str" cm="1">
+      <c r="G225" s="61" t="str" cm="1">
         <f t="array" ref="G225" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</f>
         <v>US</v>
       </c>

</xml_diff>

<commit_message>
Moved idCol0 to a different control table
Moved column `idCol0` from `co_moduleScenarios` to `co_inputInfo`
</commit_message>
<xml_diff>
--- a/inst/extdata/controlTables.xlsx
+++ b/inst/extdata/controlTables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A098C3-926A-40EC-87BE-15D09BCCE555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD36182-05FD-4DF5-AD2B-C469B567ECA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="367">
   <si>
     <t>Midwest</t>
   </si>
@@ -2280,6 +2280,31 @@
   </cellStyles>
   <dxfs count="160">
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
@@ -3100,31 +3125,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5630,68 +5630,67 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{130DC324-CB3E-4D07-B21F-C092D038DD02}" name="co_moduleScenarios" displayName="co_moduleScenarios" ref="B124:H131" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{130DC324-CB3E-4D07-B21F-C092D038DD02}" name="co_moduleScenarios" displayName="co_moduleScenarios" ref="B124:G131" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{153273EE-D49C-43E7-89D3-640CF711FDD6}" name="row_id" dataDxfId="53">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleScenarios[[#This Row],[row_id]] ) - ROW( co_moduleScenarios[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{F54B7C7D-6137-4D7A-AA53-E6EC1A4D870B}" name="inputName" dataDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{6FE2E9D8-6B04-436E-8205-1717138EBEA7}" name="idCol0" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{8C7B1E0B-A838-4C25-BD81-F2D99A20C316}" name="fredi" dataDxfId="50"/>
-    <tableColumn id="2" xr3:uid="{DE883AA6-AFB1-4ECB-81BC-2DBBBB7D9EC6}" name="sv" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{03493EE6-57B6-434B-89CB-00D18647CE1C}" name="extremes" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{FD0E66B9-364C-46F1-A441-3593D5002F5F}" name="ghg" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{8C7B1E0B-A838-4C25-BD81-F2D99A20C316}" name="fredi" dataDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{DE883AA6-AFB1-4ECB-81BC-2DBBBB7D9EC6}" name="sv" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{03493EE6-57B6-434B-89CB-00D18647CE1C}" name="extremes" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{FD0E66B9-364C-46F1-A441-3593D5002F5F}" name="ghg" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}" name="co_moduleInfo" displayName="co_moduleInfo" ref="B22:G26" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}" name="co_moduleInfo" displayName="co_moduleInfo" ref="B22:G26" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="B22:G26" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B23:G25">
     <sortCondition ref="C33:C35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1E91507F-C783-4AF1-A2DC-F0D550DB8228}" name="row_id" dataDxfId="44" totalsRowDxfId="43">
+    <tableColumn id="1" xr3:uid="{1E91507F-C783-4AF1-A2DC-F0D550DB8228}" name="row_id" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleInfo[[#This Row],[row_id]] ) - ROW(co_moduleInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C5A172CB-7A1A-40A6-B5FF-ADA60A854570}" name="module" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{40CB1771-C104-47EE-A9D3-FC2266D98E31}" name="defaultMinYr" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{361574C9-CD04-4844-8EA4-8686C22861AF}" name="defaultMaxYr" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{BE556F7A-79ED-4CF4-9DE1-89B19E392F66}" name="moduleMinYr" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{EE868D0F-708E-48BF-843C-D20D3F01FC0A}" name="moduleMaxYr" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{C5A172CB-7A1A-40A6-B5FF-ADA60A854570}" name="module" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{40CB1771-C104-47EE-A9D3-FC2266D98E31}" name="defaultMinYr" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{361574C9-CD04-4844-8EA4-8686C22861AF}" name="defaultMaxYr" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{BE556F7A-79ED-4CF4-9DE1-89B19E392F66}" name="moduleMinYr" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{EE868D0F-708E-48BF-843C-D20D3F01FC0A}" name="moduleMaxYr" dataDxfId="35" totalsRowDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3617F852-F5F0-4F60-AE1D-02F268E7E5D0}" name="co_moduleModTypes" displayName="co_moduleModTypes" ref="B69:F73" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3617F852-F5F0-4F60-AE1D-02F268E7E5D0}" name="co_moduleModTypes" displayName="co_moduleModTypes" ref="B69:F73" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B2363595-A68F-4CF5-9F7E-DD47303CE84C}" name="row_id" dataDxfId="30">
+    <tableColumn id="1" xr3:uid="{B2363595-A68F-4CF5-9F7E-DD47303CE84C}" name="row_id" dataDxfId="31">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleModTypes[[#This Row],[row_id]] ) - ROW( co_moduleModTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D18390C5-26C7-473C-9856-A402FD3A0AEF}" name="module" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{C4E5B6A3-7C3C-4259-823B-02A74FE928D8}" name="gcm" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{F47429F2-FAE8-479B-9DBC-65A9498A8337}" name="slr" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{935107B0-7729-4F94-B463-7640686C80D6}" name="gcm_ghg" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{D18390C5-26C7-473C-9856-A402FD3A0AEF}" name="module" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{C4E5B6A3-7C3C-4259-823B-02A74FE928D8}" name="gcm" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{F47429F2-FAE8-479B-9DBC-65A9498A8337}" name="slr" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{935107B0-7729-4F94-B463-7640686C80D6}" name="gcm_ghg" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{826DC812-3005-4F51-B0FF-C3E353D9AAA4}" name="co_scenarios" displayName="co_scenarios" ref="B104:G116" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{826DC812-3005-4F51-B0FF-C3E353D9AAA4}" name="co_scenarios" displayName="co_scenarios" ref="B104:G116" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6346090C-91C3-4EDB-A7F1-370F8A29D56E}" name="row_id" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{6346090C-91C3-4EDB-A7F1-370F8A29D56E}" name="row_id" dataDxfId="24">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_scenarios[[#This Row],[row_id]] ) - ROW( co_scenarios[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF567B04-BAFE-4398-9598-BABE0A898EC3}" name="scenarioName" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{11EC5AD1-152B-4E01-89B5-BF7C4B3D34E7}" name="inputName" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{713CE323-B977-4F6A-A751-4F21E1A47B9D}" name="inputArgType" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{A3EF825F-7245-45C7-97D2-FB17A58B2688}" name="inputArgVal" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{F4BED776-1DB1-4B5A-B96F-C7A6885A2CF1}" name="scenario" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{AF567B04-BAFE-4398-9598-BABE0A898EC3}" name="scenarioName" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{11EC5AD1-152B-4E01-89B5-BF7C4B3D34E7}" name="inputName" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{713CE323-B977-4F6A-A751-4F21E1A47B9D}" name="inputArgType" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{A3EF825F-7245-45C7-97D2-FB17A58B2688}" name="inputArgVal" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{F4BED776-1DB1-4B5A-B96F-C7A6885A2CF1}" name="scenario" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5701,10 +5700,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}" name="Readme_adaptations" displayName="Readme_adaptations" ref="B9:E15" totalsRowShown="0">
   <autoFilter ref="B9:E15" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="18">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_adaptations[[#This Row],[row_id]] ) - ROW( Readme_adaptations[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{13712644-0D89-49D5-9571-32BD03BF1BD3}" name="adapt_id"/>
     <tableColumn id="3" xr3:uid="{B89736B7-3040-4F82-B2CC-EB15F47F50B3}" name="adapt_label"/>
   </tableColumns>
@@ -5713,16 +5712,16 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="B3:F5" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="14">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_sectors[[#This Row],[row_id]] ) - ROW( Readme_sectors[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5732,17 +5731,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}" name="slr_cm" displayName="slr_cm" ref="A1:I102" totalsRowShown="0">
   <autoFilter ref="A1:I102" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="9">
       <calculatedColumnFormula xml:space="preserve"> ROW( slr_cm[[#This Row],[row_id]] ) - ROW( slr_cm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5877,8 +5876,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B92:M99" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B92:N99" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="95">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
@@ -5897,6 +5896,7 @@
     </tableColumn>
     <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="regional" dataDxfId="85"/>
     <tableColumn id="12" xr3:uid="{FB827980-3826-439F-9F41-FE917F82F38E}" name="groupCols" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{85CFD1EB-2080-4260-A066-309BD3B1C8B8}" name="idCol0" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6975,11 +6975,11 @@
       </c>
       <c r="K11" s="16" cm="1">
         <f t="array" aca="1" ref="K11" ca="1" xml:space="preserve"> MAX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] ) ) )</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L11" s="16">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[last_colIndex]] - doc_tablesList[[#This Row],[id_colIndex]] + 1</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M11" s="29"/>
       <c r="N11" s="28" t="s">
@@ -7067,11 +7067,11 @@
       </c>
       <c r="K13" s="16" cm="1">
         <f t="array" aca="1" ref="K13" ca="1" xml:space="preserve"> MAX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] ) ) )</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L13" s="16">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[last_colIndex]] - doc_tablesList[[#This Row],[id_colIndex]] + 1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M13" s="29"/>
       <c r="N13" s="28" t="s">
@@ -7331,9 +7331,9 @@
   </sheetPr>
   <dimension ref="A1:U227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A120" sqref="A120:XFD120"/>
+      <selection pane="topRight" activeCell="D125" sqref="D125:D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8404,6 +8404,9 @@
       <c r="M92" s="14" t="s">
         <v>361</v>
       </c>
+      <c r="N92" s="14" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B93" s="3">
@@ -8442,6 +8445,9 @@
       <c r="M93" s="13" t="s">
         <v>362</v>
       </c>
+      <c r="N93" s="13" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B94" s="3">
@@ -8480,6 +8486,9 @@
       <c r="M94" s="13" t="s">
         <v>362</v>
       </c>
+      <c r="N94" s="13" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B95" s="3">
@@ -8517,6 +8526,9 @@
         <v>0</v>
       </c>
       <c r="M95" s="13"/>
+      <c r="N95" s="13" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B96" s="3">
@@ -8556,6 +8568,9 @@
       <c r="M96" s="13" t="s">
         <v>364</v>
       </c>
+      <c r="N96" s="13" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B97" s="3">
@@ -8593,6 +8608,9 @@
         <v>0</v>
       </c>
       <c r="M97" s="13"/>
+      <c r="N97" s="13" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B98" s="3">
@@ -8630,6 +8648,9 @@
         <v>0</v>
       </c>
       <c r="M98" s="13"/>
+      <c r="N98" s="13" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B99" s="3">
@@ -8668,6 +8689,9 @@
       </c>
       <c r="M99" s="13" t="s">
         <v>363</v>
+      </c>
+      <c r="N99" s="13" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="102" spans="1:21" ht="15" x14ac:dyDescent="0.25">
@@ -8732,7 +8756,9 @@
       <c r="F105" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="G105" s="26"/>
+      <c r="G105" s="26" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B106" s="3">
@@ -8751,7 +8777,9 @@
       <c r="F106" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="G106" s="26"/>
+      <c r="G106" s="26" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B107" s="3">
@@ -8791,7 +8819,9 @@
       <c r="F108" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="G108" s="26"/>
+      <c r="G108" s="26" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B109" s="3">
@@ -8810,7 +8840,9 @@
       <c r="F109" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="G109" s="26"/>
+      <c r="G109" s="26" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B110" s="3">
@@ -8967,18 +8999,15 @@
         <v>107</v>
       </c>
       <c r="D124" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="E124" s="14" t="s">
         <v>284</v>
       </c>
+      <c r="E124" s="16" t="s">
+        <v>286</v>
+      </c>
       <c r="F124" s="16" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="G124" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="H124" s="16" t="s">
         <v>287</v>
       </c>
     </row>
@@ -8990,8 +9019,8 @@
       <c r="C125" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="D125" s="6" t="s">
-        <v>362</v>
+      <c r="D125" s="13" t="s">
+        <v>342</v>
       </c>
       <c r="E125" s="13" t="s">
         <v>342</v>
@@ -8999,10 +9028,7 @@
       <c r="F125" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="G125" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="H125" s="13"/>
+      <c r="G125" s="13"/>
     </row>
     <row r="126" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B126" s="3">
@@ -9012,8 +9038,8 @@
       <c r="C126" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D126" s="6" t="s">
-        <v>362</v>
+      <c r="D126" s="13" t="s">
+        <v>342</v>
       </c>
       <c r="E126" s="13" t="s">
         <v>342</v>
@@ -9021,10 +9047,7 @@
       <c r="F126" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="G126" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="H126" s="13"/>
+      <c r="G126" s="13"/>
     </row>
     <row r="127" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B127" s="3">
@@ -9034,8 +9057,8 @@
       <c r="C127" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D127" s="6" t="s">
-        <v>341</v>
+      <c r="D127" s="13" t="s">
+        <v>338</v>
       </c>
       <c r="E127" s="13" t="s">
         <v>338</v>
@@ -9043,10 +9066,7 @@
       <c r="F127" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="G127" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="H127" s="6" t="s">
+      <c r="G127" s="6" t="s">
         <v>338</v>
       </c>
     </row>
@@ -9059,7 +9079,7 @@
         <v>110</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>343</v>
@@ -9068,9 +9088,6 @@
         <v>343</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>343</v>
-      </c>
-      <c r="H128" s="6" t="s">
         <v>343</v>
       </c>
     </row>
@@ -9082,15 +9099,12 @@
       <c r="C129" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="D129" s="6" t="s">
-        <v>341</v>
-      </c>
+      <c r="D129" s="13"/>
       <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
+      <c r="F129" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G129" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H129" s="13" t="s">
         <v>349</v>
       </c>
     </row>
@@ -9102,15 +9116,12 @@
       <c r="C130" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>341</v>
-      </c>
+      <c r="D130" s="13"/>
       <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
+      <c r="F130" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G130" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H130" s="13" t="s">
         <v>348</v>
       </c>
     </row>
@@ -9122,15 +9133,12 @@
       <c r="C131" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="D131" s="6" t="s">
-        <v>341</v>
-      </c>
+      <c r="D131" s="13"/>
       <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
+      <c r="F131" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="G131" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H131" s="13" t="s">
         <v>350</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed GDP from SV scenarios
</commit_message>
<xml_diff>
--- a/inst/extdata/controlTables.xlsx
+++ b/inst/extdata/controlTables.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD36182-05FD-4DF5-AD2B-C469B567ECA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A10044-70CF-404A-9127-3335E551AB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15450" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="367">
   <si>
     <t>Midwest</t>
   </si>
@@ -2280,31 +2280,6 @@
   </cellStyles>
   <dxfs count="160">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <fill>
         <patternFill patternType="solid">
@@ -3713,6 +3688,31 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5581,116 +5581,116 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DFE6321-7DE3-4183-8A83-7F36C85C9DB0}" name="co_slrCm" displayName="co_slrCm" ref="B79:E86" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DFE6321-7DE3-4183-8A83-7F36C85C9DB0}" name="co_slrCm" displayName="co_slrCm" ref="B79:E86" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{3762ECAE-6A4D-4316-A236-8B365D0626D2}" name="row_id" dataDxfId="73">
+    <tableColumn id="1" xr3:uid="{3762ECAE-6A4D-4316-A236-8B365D0626D2}" name="row_id" dataDxfId="72">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_slrCm[[#This Row],[row_id]] ) - ROW( co_slrCm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{652FAEDD-ACCA-4F89-BB09-D0259DE4EBDE}" name="model" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{4E21FF99-5816-430F-A59C-839B9DED59AD}" name="model_cm" dataDxfId="71">
+    <tableColumn id="2" xr3:uid="{652FAEDD-ACCA-4F89-BB09-D0259DE4EBDE}" name="model" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{4E21FF99-5816-430F-A59C-839B9DED59AD}" name="model_cm" dataDxfId="70">
       <calculatedColumnFormula xml:space="preserve"> SUBSTITUTE( co_slrCm[[#This Row],[model]], "cm", "" )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{494DF020-2C7F-4BEC-BF92-2D1C2997DB71}" name="model_type" dataDxfId="70"/>
+    <tableColumn id="20" xr3:uid="{494DF020-2C7F-4BEC-BF92-2D1C2997DB71}" name="model_type" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D0C88C5-F2A7-46B8-8C69-B1B5A09A785D}" name="co_moduleAreas" displayName="co_moduleAreas" ref="B149:G153" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D0C88C5-F2A7-46B8-8C69-B1B5A09A785D}" name="co_moduleAreas" displayName="co_moduleAreas" ref="B149:G153" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6B39C0F6-F51F-46E7-B871-D79691468859}" name="row_id" dataDxfId="67">
+    <tableColumn id="1" xr3:uid="{6B39C0F6-F51F-46E7-B871-D79691468859}" name="row_id" dataDxfId="66">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleAreas[[#This Row],[row_id]] ) - ROW( co_moduleAreas[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FA7D71D8-3E5E-4160-8B14-D5765D9F310B}" name="module" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{FF99F0AF-3896-4181-B4BA-A7BCCD26281F}" name="CONUS" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{8D6CF49E-2833-4B79-B861-B3E559469D80}" name="AK" dataDxfId="64"/>
-    <tableColumn id="2" xr3:uid="{FBF0E9DC-EC64-4AAB-85A0-909CE7D91B5C}" name="HI" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{ECDD11B8-8AA9-466D-9A95-87825C1F011B}" name="US" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{FA7D71D8-3E5E-4160-8B14-D5765D9F310B}" name="module" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{FF99F0AF-3896-4181-B4BA-A7BCCD26281F}" name="CONUS" dataDxfId="64"/>
+    <tableColumn id="5" xr3:uid="{8D6CF49E-2833-4B79-B861-B3E559469D80}" name="AK" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{FBF0E9DC-EC64-4AAB-85A0-909CE7D91B5C}" name="HI" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{ECDD11B8-8AA9-466D-9A95-87825C1F011B}" name="US" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A7B7951-C6F2-4FD3-A1BB-7026F6A8E846}" name="co_areas" displayName="co_areas" ref="B140:E144" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0A7B7951-C6F2-4FD3-A1BB-7026F6A8E846}" name="co_areas" displayName="co_areas" ref="B140:E144" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B141:E144">
     <sortCondition ref="E141:E144"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E7EF0B14-6E39-4AC7-AF6C-1F6122F80A00}" name="row_id" dataDxfId="59">
+    <tableColumn id="1" xr3:uid="{E7EF0B14-6E39-4AC7-AF6C-1F6122F80A00}" name="row_id" dataDxfId="58">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_areas[[#This Row],[row_id]] ) - ROW( co_areas[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8E314417-76FC-49D4-8395-68E6821400F1}" name="area" dataDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{D3346EB3-CC6E-4F56-99C1-5CA14B2AA885}" name="area_label" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{49EF0AA8-E61C-4619-9F0A-C99D809CE4D7}" name="area_order" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{8E314417-76FC-49D4-8395-68E6821400F1}" name="area" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{D3346EB3-CC6E-4F56-99C1-5CA14B2AA885}" name="area_label" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{49EF0AA8-E61C-4619-9F0A-C99D809CE4D7}" name="area_order" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{130DC324-CB3E-4D07-B21F-C092D038DD02}" name="co_moduleScenarios" displayName="co_moduleScenarios" ref="B124:G131" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{130DC324-CB3E-4D07-B21F-C092D038DD02}" name="co_moduleScenarios" displayName="co_moduleScenarios" ref="B124:G131" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{153273EE-D49C-43E7-89D3-640CF711FDD6}" name="row_id" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{153273EE-D49C-43E7-89D3-640CF711FDD6}" name="row_id" dataDxfId="52">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleScenarios[[#This Row],[row_id]] ) - ROW( co_moduleScenarios[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F54B7C7D-6137-4D7A-AA53-E6EC1A4D870B}" name="inputName" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{8C7B1E0B-A838-4C25-BD81-F2D99A20C316}" name="fredi" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{DE883AA6-AFB1-4ECB-81BC-2DBBBB7D9EC6}" name="sv" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{03493EE6-57B6-434B-89CB-00D18647CE1C}" name="extremes" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{FD0E66B9-364C-46F1-A441-3593D5002F5F}" name="ghg" dataDxfId="48"/>
+    <tableColumn id="4" xr3:uid="{F54B7C7D-6137-4D7A-AA53-E6EC1A4D870B}" name="inputName" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{8C7B1E0B-A838-4C25-BD81-F2D99A20C316}" name="fredi" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{DE883AA6-AFB1-4ECB-81BC-2DBBBB7D9EC6}" name="sv" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{03493EE6-57B6-434B-89CB-00D18647CE1C}" name="extremes" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{FD0E66B9-364C-46F1-A441-3593D5002F5F}" name="ghg" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}" name="co_moduleInfo" displayName="co_moduleInfo" ref="B22:G26" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}" name="co_moduleInfo" displayName="co_moduleInfo" ref="B22:G26" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="B22:G26" xr:uid="{6E826C61-9F11-4955-B19C-8112C0F6EC23}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B23:G25">
     <sortCondition ref="C33:C35"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1E91507F-C783-4AF1-A2DC-F0D550DB8228}" name="row_id" dataDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="1" xr3:uid="{1E91507F-C783-4AF1-A2DC-F0D550DB8228}" name="row_id" dataDxfId="44" totalsRowDxfId="43">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleInfo[[#This Row],[row_id]] ) - ROW(co_moduleInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C5A172CB-7A1A-40A6-B5FF-ADA60A854570}" name="module" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{40CB1771-C104-47EE-A9D3-FC2266D98E31}" name="defaultMinYr" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{361574C9-CD04-4844-8EA4-8686C22861AF}" name="defaultMaxYr" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{BE556F7A-79ED-4CF4-9DE1-89B19E392F66}" name="moduleMinYr" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{EE868D0F-708E-48BF-843C-D20D3F01FC0A}" name="moduleMaxYr" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{C5A172CB-7A1A-40A6-B5FF-ADA60A854570}" name="module" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{40CB1771-C104-47EE-A9D3-FC2266D98E31}" name="defaultMinYr" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{361574C9-CD04-4844-8EA4-8686C22861AF}" name="defaultMaxYr" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{BE556F7A-79ED-4CF4-9DE1-89B19E392F66}" name="moduleMinYr" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{EE868D0F-708E-48BF-843C-D20D3F01FC0A}" name="moduleMaxYr" dataDxfId="34" totalsRowDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3617F852-F5F0-4F60-AE1D-02F268E7E5D0}" name="co_moduleModTypes" displayName="co_moduleModTypes" ref="B69:F73" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{3617F852-F5F0-4F60-AE1D-02F268E7E5D0}" name="co_moduleModTypes" displayName="co_moduleModTypes" ref="B69:F73" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B2363595-A68F-4CF5-9F7E-DD47303CE84C}" name="row_id" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{B2363595-A68F-4CF5-9F7E-DD47303CE84C}" name="row_id" dataDxfId="30">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_moduleModTypes[[#This Row],[row_id]] ) - ROW( co_moduleModTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D18390C5-26C7-473C-9856-A402FD3A0AEF}" name="module" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{C4E5B6A3-7C3C-4259-823B-02A74FE928D8}" name="gcm" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{F47429F2-FAE8-479B-9DBC-65A9498A8337}" name="slr" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{935107B0-7729-4F94-B463-7640686C80D6}" name="gcm_ghg" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{D18390C5-26C7-473C-9856-A402FD3A0AEF}" name="module" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{C4E5B6A3-7C3C-4259-823B-02A74FE928D8}" name="gcm" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{F47429F2-FAE8-479B-9DBC-65A9498A8337}" name="slr" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{935107B0-7729-4F94-B463-7640686C80D6}" name="gcm_ghg" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{826DC812-3005-4F51-B0FF-C3E353D9AAA4}" name="co_scenarios" displayName="co_scenarios" ref="B104:G116" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{826DC812-3005-4F51-B0FF-C3E353D9AAA4}" name="co_scenarios" displayName="co_scenarios" ref="B104:G116" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6346090C-91C3-4EDB-A7F1-370F8A29D56E}" name="row_id" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{6346090C-91C3-4EDB-A7F1-370F8A29D56E}" name="row_id" dataDxfId="23">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_scenarios[[#This Row],[row_id]] ) - ROW( co_scenarios[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AF567B04-BAFE-4398-9598-BABE0A898EC3}" name="scenarioName" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{11EC5AD1-152B-4E01-89B5-BF7C4B3D34E7}" name="inputName" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{713CE323-B977-4F6A-A751-4F21E1A47B9D}" name="inputArgType" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{A3EF825F-7245-45C7-97D2-FB17A58B2688}" name="inputArgVal" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{F4BED776-1DB1-4B5A-B96F-C7A6885A2CF1}" name="scenario" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{AF567B04-BAFE-4398-9598-BABE0A898EC3}" name="scenarioName" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{11EC5AD1-152B-4E01-89B5-BF7C4B3D34E7}" name="inputName" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{713CE323-B977-4F6A-A751-4F21E1A47B9D}" name="inputArgType" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{A3EF825F-7245-45C7-97D2-FB17A58B2688}" name="inputArgVal" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{F4BED776-1DB1-4B5A-B96F-C7A6885A2CF1}" name="scenario" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5700,10 +5700,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}" name="Readme_adaptations" displayName="Readme_adaptations" ref="B9:E15" totalsRowShown="0">
   <autoFilter ref="B9:E15" xr:uid="{0D47D4A9-4D0B-4BD8-9445-F4282AA644C2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{F4BD4BA2-1D8F-424B-9A8C-E20589922BC9}" name="row_id" dataDxfId="17">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_adaptations[[#This Row],[row_id]] ) - ROW( Readme_adaptations[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{8F8CD713-0ECF-4957-8E94-F3FC5C746031}" name="sector_id" dataDxfId="16"/>
     <tableColumn id="2" xr3:uid="{13712644-0D89-49D5-9571-32BD03BF1BD3}" name="adapt_id"/>
     <tableColumn id="3" xr3:uid="{B89736B7-3040-4F82-B2CC-EB15F47F50B3}" name="adapt_label"/>
   </tableColumns>
@@ -5712,16 +5712,16 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}" name="Readme_sectors" displayName="Readme_sectors" ref="B3:F5" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="B3:F5" xr:uid="{58C7AF19-DB28-47F8-BE56-AE985DF1009B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{055BC283-B8DC-4F37-B787-CE15D79337AE}" name="row_id" dataDxfId="13">
       <calculatedColumnFormula xml:space="preserve"> ROW( Readme_sectors[[#This Row],[row_id]] ) - ROW( Readme_sectors[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F1DE1E87-7416-4EC2-83F4-443E818D69E2}" name="sector_id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{69F42C58-EA29-416E-A03E-490DCD1DAC6F}" name="adapt_id" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{995768DD-996C-4A25-A331-EA651CF80A08}" name="adapt_label" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{B607221E-C635-413E-A992-7E4B369F50F2}" name="Description" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5731,17 +5731,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}" name="slr_cm" displayName="slr_cm" ref="A1:I102" totalsRowShown="0">
   <autoFilter ref="A1:I102" xr:uid="{1F6E1C40-0D2A-408F-87EE-36A6B84C2F85}"/>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{F80AE68D-CB1F-4EA7-B8F9-94BBA2F3B4C7}" name="row_id" dataDxfId="8">
       <calculatedColumnFormula xml:space="preserve"> ROW( slr_cm[[#This Row],[row_id]] ) - ROW( slr_cm[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FA4EDD13-4E7E-45A3-BAE3-E9197F3C6F46}" name="year" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8C03079C-35A7-401C-8DAF-080D8590CAF6}" name="0cm" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{BF06645C-1E6B-49DC-BFF3-41DC055BA794}" name="30cm" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{A579CC42-A3A8-4F15-AA9F-71AF71D9FC92}" name="50cm" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{3B78BF10-85AF-4256-B6E0-8C448D28F844}" name="100cm" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B9B22AB8-C0E3-43FA-8E5B-D07A4AB2C538}" name="150cm" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{763A0097-0CCB-4D1D-A0D6-FDF4FE810AFE}" name="200cm" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{FB0A96A9-E5BF-4003-9D05-D514A5B55CB9}" name="250cm" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5896,27 +5896,27 @@
     </tableColumn>
     <tableColumn id="9" xr3:uid="{AAA49909-67E1-4978-90ED-573C388A520B}" name="regional" dataDxfId="85"/>
     <tableColumn id="12" xr3:uid="{FB827980-3826-439F-9F41-FE917F82F38E}" name="groupCols" dataDxfId="84"/>
-    <tableColumn id="13" xr3:uid="{85CFD1EB-2080-4260-A066-309BD3B1C8B8}" name="idCol0" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{85CFD1EB-2080-4260-A066-309BD3B1C8B8}" name="idCol0" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B175:H227" totalsRowShown="0" headerRowDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B175:H227" totalsRowShown="0" headerRowDxfId="82">
   <autoFilter ref="B175:H227" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="82">
+    <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="81">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="81"/>
-    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{75C24D34-7FF1-4D85-8B86-75A1F1B7EF6C}" name="region" dataDxfId="78"/>
-    <tableColumn id="7" xr3:uid="{B0056655-B67E-486D-8580-C33D8B965DEB}" name="area" dataDxfId="77">
+    <tableColumn id="2" xr3:uid="{5B715195-2EAE-439A-84CF-1C26F65065E0}" name="state" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{42CA1BFA-BDCF-464B-91DB-4C9663461C1C}" name="postal" dataDxfId="79"/>
+    <tableColumn id="5" xr3:uid="{5807F5A8-31A9-4CC5-8FA0-243CB9917CD4}" name="fips" dataDxfId="78"/>
+    <tableColumn id="6" xr3:uid="{75C24D34-7FF1-4D85-8B86-75A1F1B7EF6C}" name="region" dataDxfId="77"/>
+    <tableColumn id="7" xr3:uid="{B0056655-B67E-486D-8580-C33D8B965DEB}" name="area" dataDxfId="76">
       <calculatedColumnFormula array="1" xml:space="preserve"> INDEX( co_regions[area], MATCH( 1, --( co_states[[#This Row],[region]] = co_regions[region] ), 0 ) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FD967E7F-5A29-4247-8725-12F353B23771}" name="state_order" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{FD967E7F-5A29-4247-8725-12F353B23771}" name="state_order" dataDxfId="75"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7331,9 +7331,9 @@
   </sheetPr>
   <dimension ref="A1:U227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D125" sqref="D125:D131"/>
+      <selection pane="topRight" activeCell="E127" sqref="E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9060,9 +9060,7 @@
       <c r="D127" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="E127" s="13" t="s">
-        <v>338</v>
-      </c>
+      <c r="E127" s="13"/>
       <c r="F127" s="13" t="s">
         <v>338</v>
       </c>

</xml_diff>